<commit_message>
Feature - Feedback button for retraining
</commit_message>
<xml_diff>
--- a/results/predictions/I Built a Self Landing Satellite.xlsx
+++ b/results/predictions/I Built a Self Landing Satellite.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F182"/>
+  <dimension ref="A1:F183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>excitement</t>
+          <t>admiration</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -3043,12 +3043,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>curiosity</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>curiosity</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -3971,12 +3971,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>excitement</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
@@ -4264,7 +4264,7 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>curiosity</t>
+          <t>excitement</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
@@ -5022,17 +5022,17 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Watch it.</t>
+          <t>Watching.</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -5635,12 +5635,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F163" t="inlineStr">
@@ -5657,22 +5657,22 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>00:13:47</t>
+          <t>00:13:46</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Can you fly back he fly up?</t>
+          <t>Can you fly back?</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F164" t="inlineStr">
@@ -5684,27 +5684,27 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
+          <t>00:13:46</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
           <t>00:13:47</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>00:13:47</t>
-        </is>
-      </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>No, it's.</t>
+          <t>He fly up?</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>neutral</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F165" t="inlineStr">
@@ -5716,27 +5716,27 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>00:13:49</t>
+          <t>00:13:47</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>00:13:52</t>
+          <t>00:13:47</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>We had a pretty rough landing due to, of all things, pilot error.</t>
+          <t>No, it's.</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>excitement</t>
+          <t>neutral</t>
         </is>
       </c>
       <c r="F166" t="inlineStr">
@@ -5748,17 +5748,17 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
+          <t>00:13:49</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
           <t>00:13:52</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>00:13:59</t>
-        </is>
-      </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>The plan was to free fall until right about 200 meters above the ground, max out the thrust, and fly back towards the launch site.</t>
+          <t>We had a pretty rough landing due to, of all things, pilot error.</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -5780,17 +5780,17 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
+          <t>00:13:52</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
           <t>00:13:59</t>
         </is>
       </c>
-      <c r="B168" t="inlineStr">
-        <is>
-          <t>00:14:06</t>
-        </is>
-      </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>But due to the stress, and because the landscape looked all the same, I didn't realize that the ground was coming until way too late.</t>
+          <t>The plan was to free fall until right about 200 meters above the ground, max out the thrust, and fly back towards the launch site.</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -5812,17 +5812,17 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
+          <t>00:13:59</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
           <t>00:14:06</t>
         </is>
       </c>
-      <c r="B169" t="inlineStr">
-        <is>
-          <t>00:14:15</t>
-        </is>
-      </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>Luckily, we knew the general location of the Cansat thanks to the onboard footage, and it only took us a mere three to four minutes before it was located.</t>
+          <t>But due to the stress, and because the landscape looked all the same, I didn't realize that the ground was coming until way too late.</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -5844,17 +5844,17 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>00:14:28</t>
+          <t>00:14:06</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>00:14:34</t>
+          <t>00:14:15</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Somehow, the Kansai was still completely intact with only slight bending in one of the arms.</t>
+          <t>Luckily, we knew the general location of the Cansat thanks to the onboard footage, and it only took us a mere three to four minutes before it was located.</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>excitement</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -5876,17 +5876,17 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
+          <t>00:14:28</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
           <t>00:14:34</t>
         </is>
       </c>
-      <c r="B171" t="inlineStr">
-        <is>
-          <t>00:14:38</t>
-        </is>
-      </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>So after getting the arms replaced, the satellite was as good as new.</t>
+          <t>Somehow, the Kansai was still completely intact with only slight bending in one of the arms.</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -5908,17 +5908,17 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
+          <t>00:14:34</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
           <t>00:14:38</t>
         </is>
       </c>
-      <c r="B172" t="inlineStr">
-        <is>
-          <t>00:14:43</t>
-        </is>
-      </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>We even managed to recover our data thanks to this single G force indicator.</t>
+          <t>So after getting the arms replaced, the satellite was as good as new.</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -5940,17 +5940,17 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
+          <t>00:14:38</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
           <t>00:14:43</t>
         </is>
       </c>
-      <c r="B173" t="inlineStr">
-        <is>
-          <t>00:14:48</t>
-        </is>
-      </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>Just make a program to grab the value from every frame, graph it over time, and do some integration.</t>
+          <t>We even managed to recover our data thanks to this single G force indicator.</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -5972,27 +5972,27 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
+          <t>00:14:43</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
           <t>00:14:48</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>00:14:50</t>
-        </is>
-      </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>And now you have altitude.</t>
+          <t>Just make a program to grab the value from every frame, graph it over time, and do some integration.</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>fear</t>
+          <t>happiness</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>nervousness</t>
+          <t>excitement</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
@@ -6004,27 +6004,27 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
+          <t>00:14:48</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
           <t>00:14:50</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>00:14:54</t>
-        </is>
-      </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>We spent the rest of the day just flying this thing around randomly for fun.</t>
+          <t>And now you have altitude.</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>happiness</t>
+          <t>fear</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>excitement</t>
+          <t>nervousness</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
@@ -6036,17 +6036,17 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
+          <t>00:14:50</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
           <t>00:14:54</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>00:14:59</t>
-        </is>
-      </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>And we also did this freefall test, and I think I'm now a much better pilot.</t>
+          <t>We spent the rest of the day just flying this thing around randomly for fun.</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -6068,17 +6068,17 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
+          <t>00:14:54</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
           <t>00:14:59</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>00:15:05</t>
-        </is>
-      </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Speaking of that, we were actually offered a second launch on a bigger and more powerful rocket in Seattle during the summer.</t>
+          <t>And we also did this freefall test, and I think I'm now a much better pilot.</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -6100,17 +6100,17 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
+          <t>00:14:59</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
           <t>00:15:05</t>
         </is>
       </c>
-      <c r="B178" t="inlineStr">
-        <is>
-          <t>00:15:09</t>
-        </is>
-      </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>So make sure to let me know in the comments if you are interested.</t>
+          <t>Speaking of that, we were actually offered a second launch on a bigger and more powerful rocket in Seattle during the summer.</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -6132,17 +6132,17 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>00:15:13</t>
+          <t>00:15:05</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>00:15:19</t>
+          <t>00:15:09</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>And with that being said, special thanks to Zach, Daniel, Emre, Eric and Cynthia for working on this project with me.</t>
+          <t>So make sure to let me know in the comments if you are interested.</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -6164,17 +6164,17 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
+          <t>00:15:13</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
           <t>00:15:19</t>
         </is>
       </c>
-      <c r="B180" t="inlineStr">
-        <is>
-          <t>00:15:23</t>
-        </is>
-      </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Special thanks to everyone at KANSAT who made this experience possible.</t>
+          <t>And with that being said, special thanks to Zach, Daniel, Emre, Eric and Cynthia for working on this project with me.</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -6196,17 +6196,17 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
+          <t>00:15:19</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
           <t>00:15:23</t>
         </is>
       </c>
-      <c r="B181" t="inlineStr">
-        <is>
-          <t>00:15:25</t>
-        </is>
-      </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>And thank you to you for watching.</t>
+          <t>Special thanks to everyone at Kansat who made this experience possible.</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -6216,7 +6216,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>admiration</t>
+          <t>excitement</t>
         </is>
       </c>
       <c r="F181" t="inlineStr">
@@ -6228,30 +6228,62 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
+          <t>00:15:23</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
           <t>00:15:25</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>And thank you to you for watching.</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>happiness</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>admiration</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>mild</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>00:15:25</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
         <is>
           <t>00:15:27</t>
         </is>
       </c>
-      <c r="C182" t="inlineStr">
+      <c r="C183" t="inlineStr">
         <is>
           <t>See you next time.</t>
         </is>
       </c>
-      <c r="D182" t="inlineStr">
+      <c r="D183" t="inlineStr">
         <is>
           <t>fear</t>
         </is>
       </c>
-      <c r="E182" t="inlineStr">
+      <c r="E183" t="inlineStr">
         <is>
           <t>nervousness</t>
         </is>
       </c>
-      <c r="F182" t="inlineStr">
+      <c r="F183" t="inlineStr">
         <is>
           <t>mild</t>
         </is>

</xml_diff>